<commit_message>
Correction of regional storage
</commit_message>
<xml_diff>
--- a/analysis/Sensitivity.xlsx
+++ b/analysis/Sensitivity.xlsx
@@ -58,15 +58,9 @@
     <t>Half storage costs for investment and variable costs</t>
   </si>
   <si>
-    <t>RES potential -30%</t>
-  </si>
-  <si>
     <t>Store all</t>
   </si>
   <si>
-    <t>RES potential +30%</t>
-  </si>
-  <si>
     <t>Double cost storage</t>
   </si>
   <si>
@@ -86,6 +80,12 @@
   </si>
   <si>
     <t>30% more area for RES necessary (e.g. 1.3 for turbine)</t>
+  </si>
+  <si>
+    <t>RES Area Use -30%</t>
+  </si>
+  <si>
+    <t>RES Area Use +30%</t>
   </si>
 </sst>
 </file>
@@ -152,9 +152,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.35802363744493204"/>
+          <c:x val="0.35802363744493215"/>
           <c:y val="2.9513661539253201E-2"/>
-          <c:w val="0.58051225677027685"/>
+          <c:w val="0.5805122567702764"/>
           <c:h val="0.42064900764048707"/>
         </c:manualLayout>
       </c:layout>
@@ -192,10 +192,10 @@
                   <c:v>Half cost storage</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>RES potential +30%</c:v>
+                  <c:v>RES Area Use -30%</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>RES potential -30%</c:v>
+                  <c:v>RES Area Use +30%</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Store all</c:v>
@@ -267,10 +267,10 @@
                   <c:v>Half cost storage</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>RES potential +30%</c:v>
+                  <c:v>RES Area Use -30%</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>RES potential -30%</c:v>
+                  <c:v>RES Area Use +30%</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Store all</c:v>
@@ -309,11 +309,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="118126848"/>
-        <c:axId val="118140928"/>
+        <c:axId val="128199680"/>
+        <c:axId val="118190848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="118126848"/>
+        <c:axId val="128199680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -336,13 +336,13 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118140928"/>
+        <c:crossAx val="118190848"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="r"/>
         <c:lblOffset val="300"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118140928"/>
+        <c:axId val="118190848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-30"/>
@@ -409,7 +409,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118126848"/>
+        <c:crossAx val="128199680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -458,10 +458,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.39232867316471082"/>
-          <c:y val="0.56780911679689983"/>
+          <c:x val="0.39232867316471115"/>
+          <c:y val="0.56780911679690005"/>
           <c:w val="0.52781365587869467"/>
-          <c:h val="0.10515672679857226"/>
+          <c:h val="0.10515672679857228"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -503,7 +503,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="93" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -825,7 +825,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -860,7 +860,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>100.95989388969799</v>
@@ -882,7 +882,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>398.73606363934698</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>203.08027688412599</v>
@@ -921,12 +921,12 @@
         <v>-0.1152991076640717</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>251.25482834095399</v>
@@ -943,12 +943,12 @@
         <v>4.12719381518313</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>337.05073901179799</v>
@@ -1034,7 +1034,17 @@
         <v>25.001131197464527</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="D13">
+        <f>D5/B19*10</f>
+        <v>0.19843736238352258</v>
+      </c>
+      <c r="E13">
+        <f>E5/C19</f>
+        <v>0.21791898377805066</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1081,7 +1091,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="B28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C28">
         <f>10/B19</f>
@@ -1090,7 +1100,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="B29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C29">
         <f>1/C19</f>
@@ -1107,7 +1117,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>